<commit_message>
only include necessary data
</commit_message>
<xml_diff>
--- a/Data/CubiTaxa.xlsx
+++ b/Data/CubiTaxa.xlsx
@@ -1,20 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10905"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://outlookuga-my.sharepoint.com/personal/ccz99536_uga_edu/Documents/Cruises/NES_CCS_Comparison/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://outlookuga-my.sharepoint.com/personal/ccz99536_uga_edu/Documents/Cruises/NES_CCS_Comparison/AcidotropicManuscript/AcidotropicDyes/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="24" documentId="8_{FEC0451C-09D2-B340-8286-1180BC448A9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3BA32AF3-F0CA-204D-B8F3-08E24A8C67DF}"/>
+  <xr:revisionPtr revIDLastSave="25" documentId="8_{FEC0451C-09D2-B340-8286-1180BC448A9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BC2E6E0E-6DC3-FA4A-8526-CF840CD660D5}"/>
   <bookViews>
-    <workbookView xWindow="14660" yWindow="920" windowWidth="15420" windowHeight="18560" activeTab="1" xr2:uid="{90E9E48E-0406-5F49-81BE-30E29CB670C6}"/>
+    <workbookView xWindow="14660" yWindow="920" windowWidth="15420" windowHeight="18560" xr2:uid="{90E9E48E-0406-5F49-81BE-30E29CB670C6}"/>
   </bookViews>
   <sheets>
     <sheet name="All" sheetId="1" r:id="rId1"/>
-    <sheet name="Diatoms" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="17">
   <si>
     <t>Treatment</t>
   </si>
@@ -85,39 +84,6 @@
   </si>
   <si>
     <t>DFB (iron chelator)</t>
-  </si>
-  <si>
-    <t>Asterionellopsis</t>
-  </si>
-  <si>
-    <t>Chaetoceros</t>
-  </si>
-  <si>
-    <t>Detonula</t>
-  </si>
-  <si>
-    <t>Minidiscus</t>
-  </si>
-  <si>
-    <t>Minutocellus</t>
-  </si>
-  <si>
-    <t>NonDiatom</t>
-  </si>
-  <si>
-    <t>Other_diatom</t>
-  </si>
-  <si>
-    <t>Pseudo nitzschia</t>
-  </si>
-  <si>
-    <t>Stephanopyxis</t>
-  </si>
-  <si>
-    <t>Thalassiosira</t>
-  </si>
-  <si>
-    <t>Genus</t>
   </si>
   <si>
     <t>SdPercentReads</t>
@@ -196,10 +162,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -521,7 +483,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC2FA492-AD98-CE4B-85DA-0AF24BFA24DD}">
   <dimension ref="A1:E55"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
@@ -541,7 +503,7 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -1460,1061 +1422,6 @@
       </c>
       <c r="E55" s="2">
         <v>3.2519920065196</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B6C6489-18F8-7846-A1CB-7BCB18F1C7CB}">
-  <dimension ref="A1:E61"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="3" max="3" width="14.33203125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>7</v>
-      </c>
-      <c r="B2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" s="2">
-        <v>5.1374257190000003</v>
-      </c>
-      <c r="E2" s="2">
-        <v>1.79007655</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>7</v>
-      </c>
-      <c r="B3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="2">
-        <v>5.705376792</v>
-      </c>
-      <c r="E3" s="2">
-        <v>2.6345934130000002</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" s="2">
-        <v>5.1259090550000002</v>
-      </c>
-      <c r="E4" s="2">
-        <v>1.9240027799999999</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>7</v>
-      </c>
-      <c r="B5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="2">
-        <v>33.079993190000003</v>
-      </c>
-      <c r="E5" s="2">
-        <v>5.3036573520000001</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>7</v>
-      </c>
-      <c r="B6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D6" s="2">
-        <v>3.809200385</v>
-      </c>
-      <c r="E6" s="2">
-        <v>2.5496836329999999</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>7</v>
-      </c>
-      <c r="B7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" s="2">
-        <v>13.28579897</v>
-      </c>
-      <c r="E7" s="2">
-        <v>7.5841956850000001</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D8" s="2">
-        <v>5.888878397</v>
-      </c>
-      <c r="E8" s="2">
-        <v>0.28058596699999999</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>7</v>
-      </c>
-      <c r="B9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D9" s="2">
-        <v>0.62591286499999998</v>
-      </c>
-      <c r="E9" s="2">
-        <v>0.405698534</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10">
-        <v>7</v>
-      </c>
-      <c r="B10" t="s">
-        <v>13</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D10" s="2">
-        <v>0.29466951299999999</v>
-      </c>
-      <c r="E10" s="2">
-        <v>3.4505689999999999E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11">
-        <v>7</v>
-      </c>
-      <c r="B11" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D11" s="2">
-        <v>27.046835120000001</v>
-      </c>
-      <c r="E11" s="2">
-        <v>11.79426387</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12">
-        <v>7</v>
-      </c>
-      <c r="B12" t="s">
-        <v>14</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D12" s="2">
-        <v>7.4163090560000002</v>
-      </c>
-      <c r="E12" s="2">
-        <v>5.6002116329999998</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13">
-        <v>7</v>
-      </c>
-      <c r="B13" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D13" s="2">
-        <v>3.8618889740000002</v>
-      </c>
-      <c r="E13" s="2">
-        <v>2.1238441309999998</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14">
-        <v>7</v>
-      </c>
-      <c r="B14" t="s">
-        <v>14</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D14" s="2">
-        <v>7.1514469329999999</v>
-      </c>
-      <c r="E14" s="2">
-        <v>1.1299067140000001</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15">
-        <v>7</v>
-      </c>
-      <c r="B15" t="s">
-        <v>14</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D15" s="2">
-        <v>29.148215839999999</v>
-      </c>
-      <c r="E15" s="2">
-        <v>6.1272180189999998</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16">
-        <v>7</v>
-      </c>
-      <c r="B16" t="s">
-        <v>14</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D16" s="2">
-        <v>2.2635122829999998</v>
-      </c>
-      <c r="E16" s="2">
-        <v>0.78528390800000003</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17">
-        <v>7</v>
-      </c>
-      <c r="B17" t="s">
-        <v>14</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D17" s="2">
-        <v>6.3343355849999998</v>
-      </c>
-      <c r="E17" s="2">
-        <v>0.70662523300000002</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18">
-        <v>7</v>
-      </c>
-      <c r="B18" t="s">
-        <v>14</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D18" s="2">
-        <v>7.295116299</v>
-      </c>
-      <c r="E18" s="2">
-        <v>0.68241763899999996</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19">
-        <v>7</v>
-      </c>
-      <c r="B19" t="s">
-        <v>14</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D19" s="2">
-        <v>0.420454149</v>
-      </c>
-      <c r="E19" s="2">
-        <v>0.158171281</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20">
-        <v>7</v>
-      </c>
-      <c r="B20" t="s">
-        <v>14</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D20" s="2">
-        <v>0.24854821799999999</v>
-      </c>
-      <c r="E20" s="2">
-        <v>4.3785633999999997E-2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21">
-        <v>7</v>
-      </c>
-      <c r="B21" t="s">
-        <v>14</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D21" s="2">
-        <v>35.860172660000003</v>
-      </c>
-      <c r="E21" s="2">
-        <v>8.6191666359999992</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22">
-        <v>7</v>
-      </c>
-      <c r="B22" t="s">
-        <v>15</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D22" s="2">
-        <v>3.4592581459999998</v>
-      </c>
-      <c r="E22" s="2">
-        <v>0.71483595300000002</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23">
-        <v>7</v>
-      </c>
-      <c r="B23" t="s">
-        <v>15</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D23" s="2">
-        <v>7.0962933000000001</v>
-      </c>
-      <c r="E23" s="2">
-        <v>1.6881996180000001</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24">
-        <v>7</v>
-      </c>
-      <c r="B24" t="s">
-        <v>15</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D24" s="2">
-        <v>0.868398318</v>
-      </c>
-      <c r="E24" s="2">
-        <v>0.32250821400000002</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25">
-        <v>7</v>
-      </c>
-      <c r="B25" t="s">
-        <v>15</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D25" s="2">
-        <v>14.90102489</v>
-      </c>
-      <c r="E25" s="2">
-        <v>4.0155345779999996</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26">
-        <v>7</v>
-      </c>
-      <c r="B26" t="s">
-        <v>15</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D26" s="2">
-        <v>2.6065266249999999</v>
-      </c>
-      <c r="E26" s="2">
-        <v>0.77541406199999996</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27">
-        <v>7</v>
-      </c>
-      <c r="B27" t="s">
-        <v>15</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D27" s="2">
-        <v>54.278682770000003</v>
-      </c>
-      <c r="E27" s="2">
-        <v>6.8815161829999996</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28">
-        <v>7</v>
-      </c>
-      <c r="B28" t="s">
-        <v>15</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D28" s="2">
-        <v>8.2434614340000003</v>
-      </c>
-      <c r="E28" s="2">
-        <v>0.76936464199999999</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29">
-        <v>7</v>
-      </c>
-      <c r="B29" t="s">
-        <v>15</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D29" s="2">
-        <v>1.0422284909999999</v>
-      </c>
-      <c r="E29" s="2">
-        <v>0.29210213699999998</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A30">
-        <v>7</v>
-      </c>
-      <c r="B30" t="s">
-        <v>15</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D30" s="2">
-        <v>2.6645654090000002</v>
-      </c>
-      <c r="E30" s="2">
-        <v>0.80957478199999999</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A31">
-        <v>7</v>
-      </c>
-      <c r="B31" t="s">
-        <v>15</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D31" s="2">
-        <v>4.8395606190000002</v>
-      </c>
-      <c r="E31" s="2">
-        <v>1.6498455299999999</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A32">
-        <v>11</v>
-      </c>
-      <c r="B32" t="s">
-        <v>13</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D32" s="2">
-        <v>1.5272306330000001</v>
-      </c>
-      <c r="E32" s="2">
-        <v>1.6031192030000001</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A33">
-        <v>11</v>
-      </c>
-      <c r="B33" t="s">
-        <v>13</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D33" s="2">
-        <v>3.2062160529999999</v>
-      </c>
-      <c r="E33" s="2">
-        <v>3.0471680999999999</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A34">
-        <v>11</v>
-      </c>
-      <c r="B34" t="s">
-        <v>13</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D34" s="2">
-        <v>0.61234244299999996</v>
-      </c>
-      <c r="E34" s="2">
-        <v>0.58377406600000004</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A35">
-        <v>11</v>
-      </c>
-      <c r="B35" t="s">
-        <v>13</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D35" s="2">
-        <v>5.0444369330000001</v>
-      </c>
-      <c r="E35" s="2">
-        <v>4.9851980510000002</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A36">
-        <v>11</v>
-      </c>
-      <c r="B36" t="s">
-        <v>13</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D36" s="2">
-        <v>0.87183623600000004</v>
-      </c>
-      <c r="E36" s="2">
-        <v>0.65732448899999996</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A37">
-        <v>11</v>
-      </c>
-      <c r="B37" t="s">
-        <v>13</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D37" s="2">
-        <v>76.319784580000004</v>
-      </c>
-      <c r="E37" s="2">
-        <v>15.552878420000001</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A38">
-        <v>11</v>
-      </c>
-      <c r="B38" t="s">
-        <v>13</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D38" s="2">
-        <v>4.8216196480000004</v>
-      </c>
-      <c r="E38" s="2">
-        <v>1.7440450489999999</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A39">
-        <v>11</v>
-      </c>
-      <c r="B39" t="s">
-        <v>13</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D39" s="2">
-        <v>0.98829102099999999</v>
-      </c>
-      <c r="E39" s="2">
-        <v>0.88393018099999998</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A40">
-        <v>11</v>
-      </c>
-      <c r="B40" t="s">
-        <v>13</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D40" s="2">
-        <v>2.8724919880000002</v>
-      </c>
-      <c r="E40" s="2">
-        <v>1.047289887</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A41">
-        <v>11</v>
-      </c>
-      <c r="B41" t="s">
-        <v>13</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D41" s="2">
-        <v>3.7357504609999999</v>
-      </c>
-      <c r="E41" s="2">
-        <v>3.229821812</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A42">
-        <v>11</v>
-      </c>
-      <c r="B42" t="s">
-        <v>14</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D42" s="2">
-        <v>1.525357099</v>
-      </c>
-      <c r="E42" s="2">
-        <v>0.15001192499999999</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A43">
-        <v>11</v>
-      </c>
-      <c r="B43" t="s">
-        <v>14</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D43" s="2">
-        <v>6.2168211759999998</v>
-      </c>
-      <c r="E43" s="2">
-        <v>2.912032602</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A44">
-        <v>11</v>
-      </c>
-      <c r="B44" t="s">
-        <v>14</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D44" s="2">
-        <v>0.68495926200000001</v>
-      </c>
-      <c r="E44" s="2">
-        <v>0.51607486800000002</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A45">
-        <v>11</v>
-      </c>
-      <c r="B45" t="s">
-        <v>14</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D45" s="2">
-        <v>7.002364697</v>
-      </c>
-      <c r="E45" s="2">
-        <v>4.1876329009999997</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A46">
-        <v>11</v>
-      </c>
-      <c r="B46" t="s">
-        <v>14</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D46" s="2">
-        <v>1.095361684</v>
-      </c>
-      <c r="E46" s="2">
-        <v>0.43268084499999998</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A47">
-        <v>11</v>
-      </c>
-      <c r="B47" t="s">
-        <v>14</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D47" s="2">
-        <v>67.150685659999994</v>
-      </c>
-      <c r="E47" s="2">
-        <v>13.44662276</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A48">
-        <v>11</v>
-      </c>
-      <c r="B48" t="s">
-        <v>14</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D48" s="2">
-        <v>5.4864585540000004</v>
-      </c>
-      <c r="E48" s="2">
-        <v>1.972861523</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A49">
-        <v>11</v>
-      </c>
-      <c r="B49" t="s">
-        <v>14</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D49" s="2">
-        <v>1.6705087709999999</v>
-      </c>
-      <c r="E49" s="2">
-        <v>1.866161296</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A50">
-        <v>11</v>
-      </c>
-      <c r="B50" t="s">
-        <v>14</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D50" s="2">
-        <v>3.4264741120000002</v>
-      </c>
-      <c r="E50" s="2">
-        <v>1.26366391</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A51">
-        <v>11</v>
-      </c>
-      <c r="B51" t="s">
-        <v>14</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D51" s="2">
-        <v>5.7410089839999996</v>
-      </c>
-      <c r="E51" s="2">
-        <v>4.4468695809999996</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A52">
-        <v>11</v>
-      </c>
-      <c r="B52" t="s">
-        <v>15</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D52" s="2">
-        <v>1.126849202</v>
-      </c>
-      <c r="E52" s="2">
-        <v>0.26184302700000001</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A53">
-        <v>11</v>
-      </c>
-      <c r="B53" t="s">
-        <v>15</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D53" s="2">
-        <v>9.3923804489999991</v>
-      </c>
-      <c r="E53" s="2">
-        <v>5.4392972149999999</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A54">
-        <v>11</v>
-      </c>
-      <c r="B54" t="s">
-        <v>15</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D54" s="2">
-        <v>0.61189824400000004</v>
-      </c>
-      <c r="E54" s="2">
-        <v>0.29320670700000001</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A55">
-        <v>11</v>
-      </c>
-      <c r="B55" t="s">
-        <v>15</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D55" s="2">
-        <v>9.7523501649999993</v>
-      </c>
-      <c r="E55" s="2">
-        <v>5.6419428580000002</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A56">
-        <v>11</v>
-      </c>
-      <c r="B56" t="s">
-        <v>15</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D56" s="2">
-        <v>2.0947351780000001</v>
-      </c>
-      <c r="E56" s="2">
-        <v>1.7896473850000001</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A57">
-        <v>11</v>
-      </c>
-      <c r="B57" t="s">
-        <v>15</v>
-      </c>
-      <c r="C57" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D57" s="2">
-        <v>52.690208149999997</v>
-      </c>
-      <c r="E57" s="2">
-        <v>5.1518676289999998</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A58">
-        <v>11</v>
-      </c>
-      <c r="B58" t="s">
-        <v>15</v>
-      </c>
-      <c r="C58" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D58" s="2">
-        <v>11.21517216</v>
-      </c>
-      <c r="E58" s="2">
-        <v>3.229777098</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A59">
-        <v>11</v>
-      </c>
-      <c r="B59" t="s">
-        <v>15</v>
-      </c>
-      <c r="C59" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D59" s="2">
-        <v>4.4801040900000002</v>
-      </c>
-      <c r="E59" s="2">
-        <v>3.0920378290000001</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A60">
-        <v>11</v>
-      </c>
-      <c r="B60" t="s">
-        <v>15</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D60" s="2">
-        <v>5.0949519250000002</v>
-      </c>
-      <c r="E60" s="2">
-        <v>5.713897534</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A61">
-        <v>11</v>
-      </c>
-      <c r="B61" t="s">
-        <v>15</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D61" s="2">
-        <v>3.5413504329999999</v>
-      </c>
-      <c r="E61" s="2">
-        <v>1.622123918</v>
       </c>
     </row>
   </sheetData>

</xml_diff>